<commit_message>
freezing add 0.2 version back
</commit_message>
<xml_diff>
--- a/test/files/example.xlsx
+++ b/test/files/example.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">'sheet1'!$A$1:$J$12</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -45,7 +48,13 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="3">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -65,7 +74,7 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -379,18 +388,151 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:10"/>
-    <row r="3" spans="1:10"/>
-    <row r="4" spans="1:10"/>
-    <row r="5" spans="1:10"/>
-    <row r="6" spans="1:10"/>
-    <row r="7" spans="1:10"/>
-    <row r="8" spans="1:10"/>
-    <row r="9" spans="1:10"/>
-    <row r="10" spans="1:10"/>
-    <row r="11" spans="1:10"/>
-    <row r="12" spans="1:10"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2"/>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>